<commit_message>
Move Table creating, formating Due Date colors and Date to own classes.
</commit_message>
<xml_diff>
--- a/Output/report.xlsx
+++ b/Output/report.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Week 36" sheetId="1" r:id="rId2"/>
+    <x:sheet name="37" sheetId="1" r:id="rId2"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -40,7 +40,7 @@
     <x:t>Top Level Assemblies</x:t>
   </x:si>
   <x:si>
-    <x:t>Josh Armstrong-Smith</x:t>
+    <x:t>Josh Smith</x:t>
   </x:si>
   <x:si>
     <x:t>CAD Files</x:t>

</xml_diff>